<commit_message>
Added rest of documentation
Added the rest of documentation, just missing the code coverage.
</commit_message>
<xml_diff>
--- a/sprints/RecipeHub Product Backlog.xlsx
+++ b/sprints/RecipeHub Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Stuff\Coding\Git\RecipeHub\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6246CB7-8665-4D56-A06E-69008BB25F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA309FA-28B1-482B-80B8-84E4238BD44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="5415" windowWidth="28080" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="-120" windowWidth="37665" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>

</xml_diff>